<commit_message>
changes to QUM, v9.1
plus PDF developed
</commit_message>
<xml_diff>
--- a/Intern Roster/Intern Roster/Test_Run_Output_v7.xlsx
+++ b/Intern Roster/Intern Roster/Test_Run_Output_v7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\SLE352 CSP\Repo\Rostering\Intern Roster\Intern Roster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E4A1EA-852F-4042-9F1F-1C424DB7B7FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D1B290-A0CE-45B9-9A70-B3799C799A88}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18380" yWindow="-110" windowWidth="18490" windowHeight="11020" firstSheet="5" activeTab="11" xr2:uid="{C23D28A7-4EDE-4825-A8EB-07F71F9D3977}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="10" xr2:uid="{C23D28A7-4EDE-4825-A8EB-07F71F9D3977}"/>
   </bookViews>
   <sheets>
     <sheet name="v7.2" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,9 @@
     <sheet name="v7.8 roster" sheetId="9" r:id="rId8"/>
     <sheet name="v7.9" sheetId="8" r:id="rId9"/>
     <sheet name="V7.9 roster" sheetId="10" r:id="rId10"/>
-    <sheet name="v7.10" sheetId="11" r:id="rId11"/>
-    <sheet name="v7.10 roster" sheetId="12" r:id="rId12"/>
+    <sheet name="v7.9 print version" sheetId="13" r:id="rId11"/>
+    <sheet name="v7.10" sheetId="11" r:id="rId12"/>
+    <sheet name="v7.10 roster" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4008" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4558" uniqueCount="28">
   <si>
     <t>Intern  (size 11)</t>
   </si>
@@ -7264,7 +7265,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C595">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C595">
     <sortCondition ref="A2:A595"/>
     <sortCondition ref="C2:C595"/>
   </sortState>
@@ -9512,6 +9513,2809 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB2BB84-DC09-48B3-B3AF-6C9412F787FC}">
+  <dimension ref="A1:O62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15">
+        <v>4</v>
+      </c>
+      <c r="F1" s="15">
+        <v>5</v>
+      </c>
+      <c r="G1" s="15">
+        <v>6</v>
+      </c>
+      <c r="H1" s="15">
+        <v>7</v>
+      </c>
+      <c r="I1" s="15">
+        <v>8</v>
+      </c>
+      <c r="J1" s="15">
+        <v>9</v>
+      </c>
+      <c r="K1" s="15">
+        <v>10</v>
+      </c>
+      <c r="L1" s="15">
+        <v>11</v>
+      </c>
+      <c r="M1" s="15">
+        <v>12</v>
+      </c>
+      <c r="N1" s="15">
+        <v>13</v>
+      </c>
+      <c r="O1" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16">
+        <v>43801</v>
+      </c>
+      <c r="C2" s="16">
+        <v>43808</v>
+      </c>
+      <c r="D2" s="16">
+        <v>43815</v>
+      </c>
+      <c r="E2" s="16">
+        <v>43822</v>
+      </c>
+      <c r="F2" s="16">
+        <v>43829</v>
+      </c>
+      <c r="G2" s="16">
+        <v>43836</v>
+      </c>
+      <c r="H2" s="16">
+        <v>43843</v>
+      </c>
+      <c r="I2" s="16">
+        <v>43850</v>
+      </c>
+      <c r="J2" s="16">
+        <v>43857</v>
+      </c>
+      <c r="K2" s="16">
+        <v>43864</v>
+      </c>
+      <c r="L2" s="16">
+        <v>43871</v>
+      </c>
+      <c r="M2" s="16">
+        <v>43878</v>
+      </c>
+      <c r="N2" s="16">
+        <v>43885</v>
+      </c>
+      <c r="O2" s="16">
+        <v>43892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>9</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>10</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>11</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="15">
+        <v>15</v>
+      </c>
+      <c r="C16" s="15">
+        <v>16</v>
+      </c>
+      <c r="D16" s="15">
+        <v>17</v>
+      </c>
+      <c r="E16" s="15">
+        <v>18</v>
+      </c>
+      <c r="F16" s="15">
+        <v>19</v>
+      </c>
+      <c r="G16" s="15">
+        <v>20</v>
+      </c>
+      <c r="H16" s="15">
+        <v>21</v>
+      </c>
+      <c r="I16" s="15">
+        <v>22</v>
+      </c>
+      <c r="J16" s="15">
+        <v>23</v>
+      </c>
+      <c r="K16" s="15">
+        <v>24</v>
+      </c>
+      <c r="L16" s="15">
+        <v>25</v>
+      </c>
+      <c r="M16" s="15">
+        <v>26</v>
+      </c>
+      <c r="N16" s="15">
+        <v>27</v>
+      </c>
+      <c r="O16" s="15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="16">
+        <v>43899</v>
+      </c>
+      <c r="C17" s="16">
+        <v>43906</v>
+      </c>
+      <c r="D17" s="16">
+        <v>43913</v>
+      </c>
+      <c r="E17" s="16">
+        <v>43920</v>
+      </c>
+      <c r="F17" s="16">
+        <v>43927</v>
+      </c>
+      <c r="G17" s="16">
+        <v>43934</v>
+      </c>
+      <c r="H17" s="16">
+        <v>43941</v>
+      </c>
+      <c r="I17" s="16">
+        <v>43948</v>
+      </c>
+      <c r="J17" s="16">
+        <v>43955</v>
+      </c>
+      <c r="K17" s="16">
+        <v>43962</v>
+      </c>
+      <c r="L17" s="16">
+        <v>43969</v>
+      </c>
+      <c r="M17" s="16">
+        <v>43976</v>
+      </c>
+      <c r="N17" s="16">
+        <v>43983</v>
+      </c>
+      <c r="O17" s="16">
+        <v>43990</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>1</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>5</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>7</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>9</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>11</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O28" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="15">
+        <v>29</v>
+      </c>
+      <c r="C35" s="15">
+        <v>30</v>
+      </c>
+      <c r="D35" s="15">
+        <v>31</v>
+      </c>
+      <c r="E35" s="15">
+        <v>32</v>
+      </c>
+      <c r="F35" s="15">
+        <v>33</v>
+      </c>
+      <c r="G35" s="15">
+        <v>34</v>
+      </c>
+      <c r="H35" s="15">
+        <v>35</v>
+      </c>
+      <c r="I35" s="15">
+        <v>36</v>
+      </c>
+      <c r="J35" s="15">
+        <v>37</v>
+      </c>
+      <c r="K35" s="15">
+        <v>38</v>
+      </c>
+      <c r="L35" s="15">
+        <v>39</v>
+      </c>
+      <c r="M35" s="15">
+        <v>40</v>
+      </c>
+      <c r="N35" s="15">
+        <v>41</v>
+      </c>
+      <c r="O35" s="15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="16">
+        <v>43997</v>
+      </c>
+      <c r="C36" s="16">
+        <v>44004</v>
+      </c>
+      <c r="D36" s="16">
+        <v>44011</v>
+      </c>
+      <c r="E36" s="16">
+        <v>44018</v>
+      </c>
+      <c r="F36" s="16">
+        <v>44025</v>
+      </c>
+      <c r="G36" s="16">
+        <v>44032</v>
+      </c>
+      <c r="H36" s="16">
+        <v>44039</v>
+      </c>
+      <c r="I36" s="16">
+        <v>44046</v>
+      </c>
+      <c r="J36" s="16">
+        <v>44053</v>
+      </c>
+      <c r="K36" s="16">
+        <v>44060</v>
+      </c>
+      <c r="L36" s="16">
+        <v>44067</v>
+      </c>
+      <c r="M36" s="16">
+        <v>44074</v>
+      </c>
+      <c r="N36" s="16">
+        <v>44081</v>
+      </c>
+      <c r="O36" s="16">
+        <v>44088</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O37" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>2</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>3</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N39" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>4</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M40" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N40" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O40" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
+        <v>5</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <v>6</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M42" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N42" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O42" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>7</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O43" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <v>8</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J44" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N44" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O44" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
+        <v>9</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L45" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M45" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N45" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O45" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
+        <v>10</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
+        <v>11</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K47" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B50" s="15">
+        <v>43</v>
+      </c>
+      <c r="C50" s="15">
+        <v>44</v>
+      </c>
+      <c r="D50" s="15">
+        <v>45</v>
+      </c>
+      <c r="E50" s="15">
+        <v>46</v>
+      </c>
+      <c r="F50" s="15">
+        <v>47</v>
+      </c>
+      <c r="G50" s="15">
+        <v>48</v>
+      </c>
+      <c r="H50" s="15">
+        <v>49</v>
+      </c>
+      <c r="I50" s="15">
+        <v>50</v>
+      </c>
+      <c r="J50" s="15">
+        <v>51</v>
+      </c>
+      <c r="K50" s="15">
+        <v>52</v>
+      </c>
+      <c r="L50" s="15">
+        <v>53</v>
+      </c>
+      <c r="M50" s="15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B51" s="16">
+        <v>44095</v>
+      </c>
+      <c r="C51" s="16">
+        <v>44102</v>
+      </c>
+      <c r="D51" s="16">
+        <v>44109</v>
+      </c>
+      <c r="E51" s="16">
+        <v>44116</v>
+      </c>
+      <c r="F51" s="16">
+        <v>44123</v>
+      </c>
+      <c r="G51" s="16">
+        <v>44130</v>
+      </c>
+      <c r="H51" s="16">
+        <v>44137</v>
+      </c>
+      <c r="I51" s="16">
+        <v>44144</v>
+      </c>
+      <c r="J51" s="16">
+        <v>44151</v>
+      </c>
+      <c r="K51" s="16">
+        <v>44158</v>
+      </c>
+      <c r="L51" s="16">
+        <v>44165</v>
+      </c>
+      <c r="M51" s="16">
+        <v>44172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="15">
+        <v>1</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
+        <v>2</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
+        <v>3</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
+        <v>4</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
+        <v>5</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="15">
+        <v>6</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J57" s="17"/>
+      <c r="K57" s="17"/>
+      <c r="L57" s="17"/>
+      <c r="M57" s="17"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
+        <v>7</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
+        <v>8</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J59" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K59" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L59" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M59" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="15">
+        <v>9</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="15">
+        <v>10</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="15">
+        <v>11</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M62" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:O3">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:O4">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:O5">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:O6">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:O7">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:O8">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9:O9">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:O10">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:O11">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:O12">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:O13">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:O18">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:O19">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:O20">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:O21">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:O22">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:O23">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:O24">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:O25">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:O26">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:O27">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:O28">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37:O37">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38:O38">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:O39">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40:O40">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41:O41">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42:O42">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43:O43">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44:O44">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45:O45">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46:O46">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47:O47">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52:I52">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53:I53">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54:I54">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B55:I55">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B56:I56">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:I57">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58:M58">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B59:M59">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60:M60">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B61:M61">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62:M62">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CIntern Roster Version 7.9&amp;RClient-friendly version</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630384C4-ECCD-46BF-AAC2-6A60A7A1B932}">
   <dimension ref="A1:C595"/>
   <sheetViews>
@@ -16067,7 +18871,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C595">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C595">
     <sortCondition ref="A2:A595"/>
     <sortCondition ref="C2:C595"/>
   </sortState>
@@ -16088,11 +18892,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2718D5-9433-462F-827B-0CC68FBBC0E2}">
   <dimension ref="A1:BC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+    <sheetView topLeftCell="AL1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -29421,7 +32225,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C595">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C595">
     <sortCondition ref="A2:A595"/>
     <sortCondition ref="C2:C595"/>
   </sortState>
@@ -41026,7 +43830,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C595">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C595">
     <sortCondition ref="A2:A595"/>
     <sortCondition ref="C2:C595"/>
   </sortState>
@@ -43276,7 +46080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87988B6D-0B21-433C-B810-E90A1164F739}">
   <dimension ref="A1:C595"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -49828,7 +52632,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C595">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C595">
     <sortCondition ref="A2:A595"/>
     <sortCondition ref="C2:C595"/>
   </sortState>
@@ -49845,5 +52649,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CIntern Roster version 7.9&amp;ROrganised CPLEX output</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>